<commit_message>
Updated Library and BOM
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5A08D0-DD67-42AE-BCFD-2718F573B9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7187D6-6B59-4DB1-9129-11C21628492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,9 +275,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -616,7 +619,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +864,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>7443551131</v>
       </c>
       <c r="B18" t="s">

</xml_diff>

<commit_message>
Finished Schematics, Libraries, and BOM
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\Electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7187D6-6B59-4DB1-9129-11C21628492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8BE9F-B75E-44BB-A653-C7645C73D8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -231,6 +231,78 @@
   </si>
   <si>
     <t>Barrel Jack Connector (14V)</t>
+  </si>
+  <si>
+    <t>STMLink Connector</t>
+  </si>
+  <si>
+    <t>UART Connector</t>
+  </si>
+  <si>
+    <t>TST-105-01-F-D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TST-105-01-F-D/9497108</t>
+  </si>
+  <si>
+    <t>SSW-106-02-TM-S-RA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/SSW-106-02-TM-S-RA/7891818</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL6330AF200Q/8032037</t>
+  </si>
+  <si>
+    <t>RST Button</t>
+  </si>
+  <si>
+    <t>TL6330AF200Q</t>
+  </si>
+  <si>
+    <t>BLM21PG600SN1D</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/BLM21PG600SN1D/584263</t>
+  </si>
+  <si>
+    <t>5988191107F</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dialight/5988191107F/1291280</t>
+  </si>
+  <si>
+    <t>LTW-170TK</t>
+  </si>
+  <si>
+    <t>White LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTW-170TK/758704</t>
+  </si>
+  <si>
+    <t>5988110107F</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dialight/5988110107F/1291272</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dialight/5988170107F/1291278</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>5988170107F</t>
   </si>
 </sst>
 </file>
@@ -616,15 +688,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -931,6 +1003,118 @@
       </c>
       <c r="F22" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -956,8 +1140,16 @@
     <hyperlink ref="F21" r:id="rId19" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
     <hyperlink ref="F22" r:id="rId20" xr:uid="{F24F68B9-18C5-460D-BD5B-59F43A82FAAF}"/>
     <hyperlink ref="F14" r:id="rId21" xr:uid="{667E62DA-33A4-46EF-93A1-57643564516A}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{B9CCDFF5-80B7-4D27-B894-4BC25F5B3571}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{1D905438-EAB5-43B5-8A1C-D637DA2CD7C6}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{75282BF4-9E9B-479A-914A-A9AEA8BA767D}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{D857A05F-43ED-4BE3-99F7-E9CBCF892FFC}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{363248AA-4FD8-4244-8D37-619F0C4D57EA}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId22"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM with Prices
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8BE9F-B75E-44BB-A653-C7645C73D8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE77FB8-FAA6-4A34-943C-7BB303389E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -303,12 +303,27 @@
   </si>
   <si>
     <t>5988170107F</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Final Total:</t>
+  </si>
+  <si>
+    <t>What we have to pay:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,12 +362,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,19 +704,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -710,8 +728,14 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -721,11 +745,18 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="3">
+        <v>14.84</v>
+      </c>
+      <c r="E2" s="3">
+        <f>$C2*$D2</f>
+        <v>14.84</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -735,11 +766,18 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E30" si="0">$C3*$D3</f>
+        <v>6.8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -749,11 +787,18 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>6.8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -763,11 +808,18 @@
       <c r="C5">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="D5" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -777,11 +829,18 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.36</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -791,11 +850,18 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="D7" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -805,11 +871,18 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="D8" s="3">
+        <v>2.58</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>5.16</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -819,11 +892,18 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="3">
+        <v>1.87</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>7.48</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -833,11 +913,18 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="D10" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -847,11 +934,18 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="D11" s="3">
+        <v>3.35</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -861,11 +955,18 @@
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="D12" s="3">
+        <v>6.26</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>25.04</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -875,11 +976,18 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="D13" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -889,11 +997,18 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="D14" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.74</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -903,11 +1018,18 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="D15" s="3">
+        <v>6.42</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>12.84</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -917,11 +1039,18 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="D16" s="3">
+        <v>2.37</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.37</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -931,11 +1060,18 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="D17" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.41</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7443551131</v>
       </c>
@@ -945,11 +1081,18 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="D18" s="3">
+        <v>3.48</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>3.48</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -959,11 +1102,18 @@
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="D19" s="3">
+        <v>3.39</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>6.78</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -973,11 +1123,18 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="D20" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -987,11 +1144,18 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="D21" s="3">
+        <v>8.67</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>17.34</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1001,11 +1165,18 @@
       <c r="C22">
         <v>6</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="D22" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1015,11 +1186,18 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="D23" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>2.68</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1029,11 +1207,18 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="D24" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -1043,11 +1228,18 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="D25" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1057,11 +1249,18 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="D26" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1071,11 +1270,18 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="D27" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1085,11 +1291,18 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="D28" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1099,11 +1312,18 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="D29" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1113,41 +1333,66 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="D30" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="3">
+        <f>SUM($E2:$E30)</f>
+        <v>134.10999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="3">
+        <f>$F$32-$E$11-$E$12-$E$23-$E$24</f>
+        <v>98.489999999999966</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D2248623-79F6-4D46-AA4B-6EF43B761FE0}"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-5.0%2FNOPB/363825?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-363825_sig-CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE" xr:uid="{1931CBDF-70C7-4F6B-9CB6-C2DBEEFCA79F}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{4D664556-4EAB-4E06-A25E-18048DDA20D2}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{72C76521-F886-40B6-9DC9-383265DAAF79}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{1D248C00-639D-482F-831C-6ADD632234C2}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{43827F98-3A79-4A80-B447-26CC33F80E06}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{58686A99-D2B2-4ABB-8E0E-E62B7705CB4F}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{9ECA8115-D7E3-47A9-8A22-A94BE94D64AC}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{423CD540-B29A-4091-92DC-786AE39243E5}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{997434B1-B835-4765-875D-6E0D70A7EF79}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{4EE1C4DA-D079-4752-B0F7-C0531C71D7C2}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{00049441-D07F-49F0-97AA-D7EA411D6E00}"/>
-    <hyperlink ref="F16" r:id="rId13" xr:uid="{EE0F79CD-B3CB-4D1B-B7CB-1541F6E9176C}"/>
-    <hyperlink ref="F17" r:id="rId14" xr:uid="{3CA6F369-FA9F-42AC-A4C2-68BDBB1DC210}"/>
-    <hyperlink ref="F18" r:id="rId15" xr:uid="{E49C395F-D830-4DC4-878B-1F55D58F82B0}"/>
-    <hyperlink ref="F19" r:id="rId16" xr:uid="{42556116-8D5B-4B48-BC82-6B043B471D47}"/>
-    <hyperlink ref="F15" r:id="rId17" xr:uid="{FDDDC4B9-964D-4700-B426-4ED6CF90C007}"/>
-    <hyperlink ref="F20" r:id="rId18" display="https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE" xr:uid="{74361421-FEE6-4D9F-A917-E742AB0C190E}"/>
-    <hyperlink ref="F21" r:id="rId19" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
-    <hyperlink ref="F22" r:id="rId20" xr:uid="{F24F68B9-18C5-460D-BD5B-59F43A82FAAF}"/>
-    <hyperlink ref="F14" r:id="rId21" xr:uid="{667E62DA-33A4-46EF-93A1-57643564516A}"/>
-    <hyperlink ref="F23" r:id="rId22" xr:uid="{B9CCDFF5-80B7-4D27-B894-4BC25F5B3571}"/>
-    <hyperlink ref="F24" r:id="rId23" xr:uid="{1D905438-EAB5-43B5-8A1C-D637DA2CD7C6}"/>
-    <hyperlink ref="F25" r:id="rId24" xr:uid="{75282BF4-9E9B-479A-914A-A9AEA8BA767D}"/>
-    <hyperlink ref="F26" r:id="rId25" xr:uid="{D857A05F-43ED-4BE3-99F7-E9CBCF892FFC}"/>
-    <hyperlink ref="F27" r:id="rId26" xr:uid="{363248AA-4FD8-4244-8D37-619F0C4D57EA}"/>
-    <hyperlink ref="F28" r:id="rId27" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
-    <hyperlink ref="F29" r:id="rId28" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
-    <hyperlink ref="F30" r:id="rId29" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D2248623-79F6-4D46-AA4B-6EF43B761FE0}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-5.0%2FNOPB/363825?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-363825_sig-CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE" xr:uid="{1931CBDF-70C7-4F6B-9CB6-C2DBEEFCA79F}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{4D664556-4EAB-4E06-A25E-18048DDA20D2}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{72C76521-F886-40B6-9DC9-383265DAAF79}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{1D248C00-639D-482F-831C-6ADD632234C2}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{43827F98-3A79-4A80-B447-26CC33F80E06}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{58686A99-D2B2-4ABB-8E0E-E62B7705CB4F}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{9ECA8115-D7E3-47A9-8A22-A94BE94D64AC}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{423CD540-B29A-4091-92DC-786AE39243E5}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{997434B1-B835-4765-875D-6E0D70A7EF79}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{4EE1C4DA-D079-4752-B0F7-C0531C71D7C2}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{00049441-D07F-49F0-97AA-D7EA411D6E00}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{EE0F79CD-B3CB-4D1B-B7CB-1541F6E9176C}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{3CA6F369-FA9F-42AC-A4C2-68BDBB1DC210}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{E49C395F-D830-4DC4-878B-1F55D58F82B0}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{42556116-8D5B-4B48-BC82-6B043B471D47}"/>
+    <hyperlink ref="G15" r:id="rId17" xr:uid="{FDDDC4B9-964D-4700-B426-4ED6CF90C007}"/>
+    <hyperlink ref="G20" r:id="rId18" display="https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE" xr:uid="{74361421-FEE6-4D9F-A917-E742AB0C190E}"/>
+    <hyperlink ref="G21" r:id="rId19" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
+    <hyperlink ref="G22" r:id="rId20" xr:uid="{F24F68B9-18C5-460D-BD5B-59F43A82FAAF}"/>
+    <hyperlink ref="G14" r:id="rId21" xr:uid="{667E62DA-33A4-46EF-93A1-57643564516A}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{B9CCDFF5-80B7-4D27-B894-4BC25F5B3571}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{1D905438-EAB5-43B5-8A1C-D637DA2CD7C6}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{75282BF4-9E9B-479A-914A-A9AEA8BA767D}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{D857A05F-43ED-4BE3-99F7-E9CBCF892FFC}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{363248AA-4FD8-4244-8D37-619F0C4D57EA}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
+    <hyperlink ref="G29" r:id="rId28" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>

</xml_diff>

<commit_message>
Created board layout, updated schematic on Buck Capacitors, Updated BOM, Updated Library
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE77FB8-FAA6-4A34-943C-7BB303389E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2681374-1F48-4CE9-8D04-ABEEF66C112A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-5.0%2FNOPB/363825?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-363825_sig-CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE</t>
   </si>
   <si>
-    <t>UUD1H150MCL1GS</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nichicon/UUD1H150MCL1GS/590040</t>
-  </si>
-  <si>
     <t>STM Chip</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>15 uF Cap</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/nichicon/UWP1HR47MCL1GB/2550802</t>
-  </si>
-  <si>
     <t>0.47uF Cap</t>
   </si>
   <si>
@@ -74,9 +65,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>UWP1HR47MCL1GB</t>
-  </si>
-  <si>
     <t>VS-6TQ045S-M3</t>
   </si>
   <si>
@@ -89,15 +77,6 @@
     <t>22uH Inductor</t>
   </si>
   <si>
-    <t>UCZ1J181MNJ1MS</t>
-  </si>
-  <si>
-    <t>180uF Cap</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nichicon/UCZ1J181MNJ1MS/5144110</t>
-  </si>
-  <si>
     <t>GRM2195C1H103JA01D</t>
   </si>
   <si>
@@ -315,6 +294,27 @@
   </si>
   <si>
     <t>What we have to pay:</t>
+  </si>
+  <si>
+    <t>TR3E156M050C0300</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-sprague/TR3E156M050C0300/2259941</t>
+  </si>
+  <si>
+    <t>100uF Cap</t>
+  </si>
+  <si>
+    <t>TPSC107K010R0200</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kyocera-avx/TPSC107K010R0200/946529</t>
+  </si>
+  <si>
+    <t>293D474X9050B2TE3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-sprague/293D474X9050B2TE3/1578900</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,27 +720,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>14.84</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -795,57 +795,57 @@
         <v>6.8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>0.48</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>2.88</v>
+        <v>11.6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>1.36</v>
+        <v>1.38</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -858,15 +858,15 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -879,36 +879,36 @@
         <v>5.16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
-        <v>1.87</v>
+        <v>0.82</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>7.48</v>
+        <v>4.92</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -921,15 +921,15 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -942,15 +942,15 @@
         <v>6.7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -963,15 +963,15 @@
         <v>25.04</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -984,15 +984,15 @@
         <v>0.69</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1005,15 +1005,15 @@
         <v>0.74</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1026,15 +1026,15 @@
         <v>12.84</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1047,15 +1047,15 @@
         <v>2.37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1068,7 +1068,7 @@
         <v>0.41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>7443551131</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1089,15 +1089,15 @@
         <v>3.48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1110,15 +1110,15 @@
         <v>6.78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1131,15 +1131,15 @@
         <v>1.72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1152,15 +1152,15 @@
         <v>17.34</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>6</v>
@@ -1173,15 +1173,15 @@
         <v>1.26</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1194,15 +1194,15 @@
         <v>2.68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1215,15 +1215,15 @@
         <v>1.2</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1236,15 +1236,15 @@
         <v>0.88</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1257,15 +1257,15 @@
         <v>0.12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1278,15 +1278,15 @@
         <v>0.59</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1299,15 +1299,15 @@
         <v>0.61</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1320,15 +1320,15 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1341,25 +1341,25 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F32" s="3">
         <f>SUM($E2:$E30)</f>
-        <v>134.10999999999999</v>
+        <v>140.29</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F33" s="3">
         <f>$F$32-$E$11-$E$12-$E$23-$E$24</f>
-        <v>98.489999999999966</v>
+        <v>104.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Schematic, board layout, BOM, and libraries
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2681374-1F48-4CE9-8D04-ABEEF66C112A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497C11AE-4F80-4AAB-87FF-A549C2FE14B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -86,15 +86,6 @@
     <t>0.01uF Cap (0805)</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-3-3-NOPB/366918</t>
-  </si>
-  <si>
-    <t>LM2678S-3.3/NOPB</t>
-  </si>
-  <si>
-    <t>3.3V Buck Controller</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32F207VGT6TR/4357621</t>
   </si>
   <si>
@@ -315,6 +306,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/vishay-sprague/293D474X9050B2TE3/1578900</t>
+  </si>
+  <si>
+    <t>3.3V LDO</t>
+  </si>
+  <si>
+    <t>TLV1117LV33DCYR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TLV1117LV33DCYR/2666508</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/runic-technology/RS0104YQ/14544678</t>
+  </si>
+  <si>
+    <t>Level Shifter</t>
+  </si>
+  <si>
+    <t>RS0104YQ</t>
   </si>
 </sst>
 </file>
@@ -704,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,15 +738,15 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -753,7 +762,7 @@
         <v>14.84</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,7 +779,7 @@
         <v>6.8</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E30" si="0">$C3*$D3</f>
+        <f t="shared" ref="E3:E31" si="0">$C3*$D3</f>
         <v>6.8</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -779,65 +788,65 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>6.8</v>
+        <v>0.35</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>6.8</v>
+        <v>0.35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>2.3199999999999998</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>11.6</v>
+        <v>6.9599999999999991</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
         <v>0.69</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>1.38</v>
+        <v>0.69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,14 +857,14 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <v>1.1299999999999999</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>2.2599999999999998</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
@@ -863,44 +872,44 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <v>2.58</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>5.16</v>
+        <v>2.58</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3">
         <v>0.82</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>4.92</v>
+        <v>2.46</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -911,14 +920,14 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
         <v>0.25</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -926,10 +935,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -942,15 +951,15 @@
         <v>6.7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -963,15 +972,15 @@
         <v>25.04</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -984,15 +993,15 @@
         <v>0.69</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1005,15 +1014,15 @@
         <v>0.74</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1026,15 +1035,15 @@
         <v>12.84</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1047,15 +1056,15 @@
         <v>2.37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1068,7 +1077,7 @@
         <v>0.41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1085,7 @@
         <v>7443551131</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1089,15 +1098,15 @@
         <v>3.48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1110,15 +1119,15 @@
         <v>6.78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1131,15 +1140,15 @@
         <v>1.72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1152,15 +1161,15 @@
         <v>17.34</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>6</v>
@@ -1173,15 +1182,15 @@
         <v>1.26</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1194,15 +1203,15 @@
         <v>2.68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1215,15 +1224,15 @@
         <v>1.2</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1236,15 +1245,15 @@
         <v>0.88</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1257,15 +1266,15 @@
         <v>0.12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1278,15 +1287,15 @@
         <v>0.59</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1299,15 +1308,15 @@
         <v>0.61</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1320,15 +1329,15 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1341,25 +1350,46 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="3">
-        <f>SUM($E2:$E30)</f>
-        <v>140.29</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>2.68</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F33" s="3">
-        <f>$F$32-$E$11-$E$12-$E$23-$E$24</f>
-        <v>104.67</v>
+        <f>SUM($E2:$E31)</f>
+        <v>124.77000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="3">
+        <f>$F$33-$E$11-$E$12-$E$23-$E$24</f>
+        <v>89.150000000000048</v>
       </c>
     </row>
   </sheetData>
@@ -1393,8 +1423,9 @@
     <hyperlink ref="G28" r:id="rId27" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
     <hyperlink ref="G29" r:id="rId28" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
     <hyperlink ref="G30" r:id="rId29" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{B194D8CE-CB58-4DF1-B97B-1B6DA0B5B044}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Power Circuit Schematic + Layout + Components
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EE5D33-F1E8-4C7E-A89D-F0E1F767712B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4566CD-2344-41E6-862D-181544EA48C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -104,30 +104,6 @@
     <t>PJ-202AH</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS63700DRCR/1672393</t>
-  </si>
-  <si>
-    <t>Inverting Boost Converter</t>
-  </si>
-  <si>
-    <t>TPS63700DRCR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/SL03-GS18/4871689</t>
-  </si>
-  <si>
-    <t>Inv Boost Con. Diode</t>
-  </si>
-  <si>
-    <t>SL03-GS18</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7443551131/1638545</t>
-  </si>
-  <si>
-    <t>Inv Boost Con. Inductor</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/bourns-inc/3352T-1-203LF/1088346</t>
   </si>
   <si>
@@ -315,6 +291,52 @@
   </si>
   <si>
     <t>330uF Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+LM43601PWPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -15V Boost Inverter</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM43601PWPR/4965739?s=N4IgTCBcDaIDoBcAEAZAsgFgMwDYAMAjAAoDqRASiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>VLS201610CX-220M-1</t>
+  </si>
+  <si>
+    <t>22uH Inductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/VLS201610CX-220M-1/5169796</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UWD1V680MCL1GS/3963027</t>
+  </si>
+  <si>
+    <t>UWD1V680MCL1GS</t>
+  </si>
+  <si>
+    <t>68uF Capacitor</t>
+  </si>
+  <si>
+    <t>ERJ-P06J681V</t>
+  </si>
+  <si>
+    <t>680 Ohm 1/2W Resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-P06J681V/525296</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-P06J561V/525286</t>
+  </si>
+  <si>
+    <t>560 Ohm 1/2W Resistor</t>
+  </si>
+  <si>
+    <t>ERJ-P06J561V</t>
   </si>
 </sst>
 </file>
@@ -362,13 +384,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -704,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,10 +754,10 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -779,10 +804,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -795,15 +820,15 @@
         <v>0.35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -816,12 +841,12 @@
         <v>1.39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -833,7 +858,7 @@
         <v>0.61</v>
       </c>
       <c r="E6" s="3">
-        <f>$C6*$D6</f>
+        <f t="shared" ref="E6:E34" si="1">$C6*$D6</f>
         <v>0.61</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -842,10 +867,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -854,19 +879,19 @@
         <v>1.55</v>
       </c>
       <c r="E7" s="3">
-        <f>$C7*$D7</f>
+        <f t="shared" si="1"/>
         <v>1.55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -875,11 +900,11 @@
         <v>1.86</v>
       </c>
       <c r="E8" s="3">
-        <f>$C8*$D8</f>
+        <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,7 +921,7 @@
         <v>0.25</v>
       </c>
       <c r="E9" s="3">
-        <f>$C9*$D9</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -917,7 +942,7 @@
         <v>3.35</v>
       </c>
       <c r="E10" s="3">
-        <f>$C10*$D10</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -938,7 +963,7 @@
         <v>6.26</v>
       </c>
       <c r="E11" s="3">
-        <f>$C11*$D11</f>
+        <f t="shared" si="1"/>
         <v>25.04</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -950,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -959,7 +984,7 @@
         <v>0.69</v>
       </c>
       <c r="E12" s="3">
-        <f>$C12*$D12</f>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -968,10 +993,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -980,19 +1005,19 @@
         <v>0.74</v>
       </c>
       <c r="E13" s="3">
-        <f>$C13*$D13</f>
+        <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1001,82 +1026,82 @@
         <v>6.42</v>
       </c>
       <c r="E14" s="3">
-        <f>$C14*$D14</f>
+        <f t="shared" si="1"/>
         <v>12.84</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>2.37</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="E15" s="3">
-        <f>$C15*$D15</f>
-        <v>2.37</v>
+        <f t="shared" si="1"/>
+        <v>4.1500000000000004</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="E16" s="3">
-        <f>$C16*$D16</f>
-        <v>0.41</v>
+        <f t="shared" si="1"/>
+        <v>0.35</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>7443551131</v>
+      <c r="A17" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>3.48</v>
+        <v>0.53</v>
       </c>
       <c r="E17" s="3">
-        <f>$C17*$D17</f>
-        <v>3.48</v>
+        <f t="shared" si="1"/>
+        <v>0.53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1085,19 +1110,19 @@
         <v>3.39</v>
       </c>
       <c r="E18" s="3">
-        <f>$C18*$D18</f>
+        <f t="shared" si="1"/>
         <v>6.78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1106,19 +1131,19 @@
         <v>0.86</v>
       </c>
       <c r="E19" s="3">
-        <f>$C19*$D19</f>
+        <f t="shared" si="1"/>
         <v>1.72</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1127,19 +1152,19 @@
         <v>8.67</v>
       </c>
       <c r="E20" s="3">
-        <f>$C20*$D20</f>
+        <f t="shared" si="1"/>
         <v>17.34</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1148,19 +1173,19 @@
         <v>0.21</v>
       </c>
       <c r="E21" s="3">
-        <f>$C21*$D21</f>
+        <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1169,19 +1194,19 @@
         <v>2.68</v>
       </c>
       <c r="E22" s="3">
-        <f>$C22*$D22</f>
+        <f t="shared" si="1"/>
         <v>2.68</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1190,19 +1215,19 @@
         <v>1.2</v>
       </c>
       <c r="E23" s="3">
-        <f>$C23*$D23</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1211,19 +1236,19 @@
         <v>0.88</v>
       </c>
       <c r="E24" s="3">
-        <f>$C24*$D24</f>
+        <f t="shared" si="1"/>
         <v>0.88</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1232,19 +1257,19 @@
         <v>0.12</v>
       </c>
       <c r="E25" s="3">
-        <f>$C25*$D25</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1253,19 +1278,19 @@
         <v>0.59</v>
       </c>
       <c r="E26" s="3">
-        <f>$C26*$D26</f>
+        <f t="shared" si="1"/>
         <v>0.59</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1274,19 +1299,19 @@
         <v>0.61</v>
       </c>
       <c r="E27" s="3">
-        <f>$C27*$D27</f>
+        <f t="shared" si="1"/>
         <v>0.61</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1295,19 +1320,19 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E28" s="3">
-        <f>$C28*$D28</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1316,19 +1341,19 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E29" s="3">
-        <f>$C29*$D29</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1337,29 +1362,83 @@
         <v>0.67</v>
       </c>
       <c r="E30" s="3">
-        <f>$C30*$D30</f>
+        <f t="shared" si="1"/>
         <v>2.68</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>0.13</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>0.13</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="3">
-        <f>SUM($E2:$E30)</f>
-        <v>116.36000000000004</v>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>76</v>
-      </c>
-      <c r="F34" s="3">
-        <f>$F$33-$E$10-$E$11-$E$22-$E$23</f>
-        <v>80.740000000000023</v>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="3">
+        <f>SUM($E2:$E34)</f>
+        <v>115.39000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="3">
+        <f>$F$36-$E$10-$E$11-$E$22-$E$23</f>
+        <v>79.770000000000024</v>
       </c>
     </row>
   </sheetData>
@@ -1375,26 +1454,25 @@
     <hyperlink ref="G10" r:id="rId9" xr:uid="{997434B1-B835-4765-875D-6E0D70A7EF79}"/>
     <hyperlink ref="G11" r:id="rId10" xr:uid="{4EE1C4DA-D079-4752-B0F7-C0531C71D7C2}"/>
     <hyperlink ref="G12" r:id="rId11" xr:uid="{00049441-D07F-49F0-97AA-D7EA411D6E00}"/>
-    <hyperlink ref="G15" r:id="rId12" xr:uid="{EE0F79CD-B3CB-4D1B-B7CB-1541F6E9176C}"/>
-    <hyperlink ref="G16" r:id="rId13" xr:uid="{3CA6F369-FA9F-42AC-A4C2-68BDBB1DC210}"/>
-    <hyperlink ref="G17" r:id="rId14" xr:uid="{E49C395F-D830-4DC4-878B-1F55D58F82B0}"/>
-    <hyperlink ref="G18" r:id="rId15" xr:uid="{42556116-8D5B-4B48-BC82-6B043B471D47}"/>
-    <hyperlink ref="G14" r:id="rId16" xr:uid="{FDDDC4B9-964D-4700-B426-4ED6CF90C007}"/>
-    <hyperlink ref="G19" r:id="rId17" display="https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE" xr:uid="{74361421-FEE6-4D9F-A917-E742AB0C190E}"/>
-    <hyperlink ref="G20" r:id="rId18" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
-    <hyperlink ref="G21" r:id="rId19" xr:uid="{F24F68B9-18C5-460D-BD5B-59F43A82FAAF}"/>
-    <hyperlink ref="G13" r:id="rId20" xr:uid="{667E62DA-33A4-46EF-93A1-57643564516A}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{B9CCDFF5-80B7-4D27-B894-4BC25F5B3571}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{1D905438-EAB5-43B5-8A1C-D637DA2CD7C6}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{75282BF4-9E9B-479A-914A-A9AEA8BA767D}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{D857A05F-43ED-4BE3-99F7-E9CBCF892FFC}"/>
-    <hyperlink ref="G26" r:id="rId25" xr:uid="{363248AA-4FD8-4244-8D37-619F0C4D57EA}"/>
-    <hyperlink ref="G27" r:id="rId26" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
-    <hyperlink ref="G28" r:id="rId27" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
-    <hyperlink ref="G29" r:id="rId28" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{B194D8CE-CB58-4DF1-B97B-1B6DA0B5B044}"/>
+    <hyperlink ref="G18" r:id="rId12" xr:uid="{42556116-8D5B-4B48-BC82-6B043B471D47}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{FDDDC4B9-964D-4700-B426-4ED6CF90C007}"/>
+    <hyperlink ref="G19" r:id="rId14" display="https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE" xr:uid="{74361421-FEE6-4D9F-A917-E742AB0C190E}"/>
+    <hyperlink ref="G20" r:id="rId15" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
+    <hyperlink ref="G21" r:id="rId16" xr:uid="{F24F68B9-18C5-460D-BD5B-59F43A82FAAF}"/>
+    <hyperlink ref="G13" r:id="rId17" xr:uid="{667E62DA-33A4-46EF-93A1-57643564516A}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{B9CCDFF5-80B7-4D27-B894-4BC25F5B3571}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{1D905438-EAB5-43B5-8A1C-D637DA2CD7C6}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{75282BF4-9E9B-479A-914A-A9AEA8BA767D}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{D857A05F-43ED-4BE3-99F7-E9CBCF892FFC}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{363248AA-4FD8-4244-8D37-619F0C4D57EA}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{01B834E2-70E7-484F-A7F8-343103F20418}"/>
+    <hyperlink ref="G28" r:id="rId24" xr:uid="{8C53AC82-9047-4D9C-A4E9-40E0927BE744}"/>
+    <hyperlink ref="G29" r:id="rId25" xr:uid="{283457BA-3B80-4E7D-BC1F-414A3454141F}"/>
+    <hyperlink ref="G30" r:id="rId26" xr:uid="{B194D8CE-CB58-4DF1-B97B-1B6DA0B5B044}"/>
+    <hyperlink ref="G31" r:id="rId27" xr:uid="{F4D0DA21-8640-40A0-9D92-CFA976672543}"/>
+    <hyperlink ref="G32" r:id="rId28" xr:uid="{F7337767-9958-4017-8D0C-E8A236D1E85C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Schematic and Board with a few components
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4566CD-2344-41E6-862D-181544EA48C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9319E55E-9488-485A-A77D-3691F8F34B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -337,6 +337,204 @@
   </si>
   <si>
     <t>ERJ-P06J561V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-(fci)/DD50P564GTXLF/4269156?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-4269156_sig-CjwKCAiA2pyuBhBKEiwApLaIO2M3EPMps9sf6SJgmdwzpmJY5_Yn4fesIPauyNWU03JmhkHHZ_yExRoCLeQQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA2pyuBhBKEiwApLaIO2M3EPMps9sf6SJgmdwzpmJY5_Yn4fesIPauyNWU03JmhkHHZ_yExRoCLeQQAvD_BwE</t>
+  </si>
+  <si>
+    <t>DD50P564GTXLF</t>
+  </si>
+  <si>
+    <t>50 Pin Analog Connector</t>
+  </si>
+  <si>
+    <t>75k Resistor</t>
+  </si>
+  <si>
+    <t>105k Resistor</t>
+  </si>
+  <si>
+    <t>73.2k Resistor</t>
+  </si>
+  <si>
+    <t>1M Resistor</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>100 Resistor</t>
+  </si>
+  <si>
+    <t>75 Resistor</t>
+  </si>
+  <si>
+    <t>330 Resistor</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>0.1u Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>1u Capacitor</t>
+  </si>
+  <si>
+    <t>4.7u Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>2.2u Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>470n Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>120p Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>10p Capacitor</t>
+  </si>
+  <si>
+    <t>10u Capacitor (X7R)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT75K0/1760535</t>
+  </si>
+  <si>
+    <t>RMCF0805FT75K0</t>
+  </si>
+  <si>
+    <t>25.5k Resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT25K5/1712905</t>
+  </si>
+  <si>
+    <t>RMCF0805FT25K5</t>
+  </si>
+  <si>
+    <t>RMCF0805FT105K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT105K/1712620</t>
+  </si>
+  <si>
+    <t>CRCW080573K2FKEA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/CRCW080573K2FKEA/1175850</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1M00</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT1M00/1760080</t>
+  </si>
+  <si>
+    <t>88.7k Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0805FT88K7</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT88K7/1713411</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
+  </si>
+  <si>
+    <t>RA73F2A2K26BTD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/RA73F2A2K26BTD/16031415</t>
+  </si>
+  <si>
+    <t>2.25k Resistor (1W)</t>
+  </si>
+  <si>
+    <t>RMCF0805FT100R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT100R/1760711</t>
+  </si>
+  <si>
+    <t>RMCF0805FT75R0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT75R0/1760492</t>
+  </si>
+  <si>
+    <t>RMCF0805FT330R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT330R/1760484</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT499R/1760282</t>
+  </si>
+  <si>
+    <t>RMCF0805FT499R</t>
+  </si>
+  <si>
+    <t>499 Resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT1K00/1760090</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1K00</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B104KCFNNNE/5961324</t>
+  </si>
+  <si>
+    <t>CL21B104KCFNNNE</t>
+  </si>
+  <si>
+    <t>CL21C100CBANNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21C100CBANNNC/3888219</t>
+  </si>
+  <si>
+    <t>CL21B105KBFNNNE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B105KBFNNNE/3886687</t>
+  </si>
+  <si>
+    <t>CL21A475KBQNNNE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A475KBQNNNE/3886906</t>
+  </si>
+  <si>
+    <t>CL21A225KB9LNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A225KB9LNNC/3888067</t>
+  </si>
+  <si>
+    <t>CL21B474KBFNNNE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B474KBFNNNE/3886697</t>
+  </si>
+  <si>
+    <t>CL21C121JDCNNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21C121JDCNNNC/3886859</t>
+  </si>
+  <si>
+    <t>CL21A106KAYNNNE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A106KAYNNNE/3888549</t>
   </si>
 </sst>
 </file>
@@ -729,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,14 +1218,14 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
         <v>6.42</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="1"/>
-        <v>12.84</v>
+        <v>6.42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>26</v>
@@ -1104,14 +1302,14 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>3.39</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="1"/>
-        <v>6.78</v>
+        <v>3.39</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
@@ -1411,34 +1609,484 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>5.82</v>
+      </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
+        <v>11.64</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="3">
+        <f>$C35*$D35</f>
+        <v>0.8</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E36" s="3">
+        <f>$C36*$D36</f>
+        <v>0.9</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E37" s="3">
+        <f>$C37*$D37</f>
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E38" s="3">
+        <f>$C38*$D38</f>
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E39" s="3">
+        <f>$C39*$D39</f>
+        <v>0.1</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E40" s="3">
+        <f>$C40*$D40</f>
+        <v>0.1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E41" s="3">
+        <f>$C41*$D41</f>
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="E42" s="3">
+        <f>$C42*$D42</f>
+        <v>7.98</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="3">
+        <f>$C43*$D43</f>
+        <v>0.1</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E44" s="3">
+        <f>$C44*$D44</f>
+        <v>0.1</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="3">
+        <f>$C45*$D45</f>
+        <v>0.8</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="3">
+        <f>$C46*$D46</f>
+        <v>0.8</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E47" s="3">
+        <f>$C47*$D47</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48">
+        <v>29</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E48" s="3">
+        <f>$C48*$D48</f>
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="3">
+        <f>$C49*$D49</f>
+        <v>0.1</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E50" s="3">
+        <f>$C50*$D50</f>
+        <v>0.75</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E51" s="3">
+        <f>$C51*$D51</f>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="E52" s="3">
+        <f>$C52*$D52</f>
+        <v>0.81</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E53" s="3">
+        <f>$C53*$D53</f>
+        <v>0.1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E54" s="3">
+        <f>$C54*$D54</f>
+        <v>0.1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="E55" s="3">
+        <f>$C55*$D55</f>
+        <v>0.18</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
         <v>67</v>
       </c>
-      <c r="F36" s="3">
-        <f>SUM($E2:$E34)</f>
-        <v>115.39000000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
+      <c r="F59" s="3">
+        <f>SUM($E2:$E55)</f>
+        <v>134.113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="3">
-        <f>$F$36-$E$10-$E$11-$E$22-$E$23</f>
-        <v>79.770000000000024</v>
+      <c r="F60" s="3">
+        <f>$F$59-$E$10-$E$11-$E$22-$E$23</f>
+        <v>98.492999999999981</v>
       </c>
     </row>
   </sheetData>
@@ -1471,8 +2119,30 @@
     <hyperlink ref="G30" r:id="rId26" xr:uid="{B194D8CE-CB58-4DF1-B97B-1B6DA0B5B044}"/>
     <hyperlink ref="G31" r:id="rId27" xr:uid="{F4D0DA21-8640-40A0-9D92-CFA976672543}"/>
     <hyperlink ref="G32" r:id="rId28" xr:uid="{F7337767-9958-4017-8D0C-E8A236D1E85C}"/>
+    <hyperlink ref="G33" r:id="rId29" display="https://www.digikey.com/en/products/detail/amphenol-icc-(fci)/DD50P564GTXLF/4269156?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-4269156_sig-CjwKCAiA2pyuBhBKEiwApLaIO2M3EPMps9sf6SJgmdwzpmJY5_Yn4fesIPauyNWU03JmhkHHZ_yExRoCLeQQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA2pyuBhBKEiwApLaIO2M3EPMps9sf6SJgmdwzpmJY5_Yn4fesIPauyNWU03JmhkHHZ_yExRoCLeQQAvD_BwE" xr:uid="{C4AC6734-FB1B-41BA-BF9D-F94A8199D869}"/>
+    <hyperlink ref="G36" r:id="rId30" xr:uid="{CD64D791-5372-4686-B9C3-D18C2C1636EF}"/>
+    <hyperlink ref="G35" r:id="rId31" xr:uid="{FCB0C861-9CB6-4CEB-AD57-38188A44BA18}"/>
+    <hyperlink ref="G37" r:id="rId32" xr:uid="{D0DE28F5-4243-473C-8437-D2B4F6C2B7FF}"/>
+    <hyperlink ref="G38" r:id="rId33" xr:uid="{9BD13656-CDD5-4347-BCB4-B02E02AAF190}"/>
+    <hyperlink ref="G39" r:id="rId34" xr:uid="{3922ACDD-8004-47CF-942C-543E6A958AB5}"/>
+    <hyperlink ref="G40" r:id="rId35" xr:uid="{472BB7B4-6AEC-45C9-B123-DE1CB165A1EE}"/>
+    <hyperlink ref="G41" r:id="rId36" xr:uid="{FF9B9C04-8BA3-4361-BB18-D8EEDFAB7E82}"/>
+    <hyperlink ref="G42" r:id="rId37" xr:uid="{E4013C94-FBE3-4BA3-9F64-EC5E0193F2DF}"/>
+    <hyperlink ref="G43" r:id="rId38" xr:uid="{2AFEA1E5-1374-481D-BF8B-FCB5EE8021DD}"/>
+    <hyperlink ref="G44" r:id="rId39" xr:uid="{B38EF415-D4B3-4EAF-93C5-668E51327084}"/>
+    <hyperlink ref="G45" r:id="rId40" xr:uid="{0E8684E1-DE64-49A2-992D-525ADCD1B6BD}"/>
+    <hyperlink ref="G46" r:id="rId41" xr:uid="{62FC5FA7-5958-4717-BEF5-65686A9E6BA7}"/>
+    <hyperlink ref="G47" r:id="rId42" xr:uid="{790B4D8F-7B98-48BF-9722-3A5AE3ACBEEE}"/>
+    <hyperlink ref="G48" r:id="rId43" xr:uid="{D2445D71-1A0A-4DFD-B705-8D45F132A76D}"/>
+    <hyperlink ref="G49" r:id="rId44" xr:uid="{D3AE4F19-1A84-4A65-BF17-24FE2E2C78F1}"/>
+    <hyperlink ref="G50" r:id="rId45" xr:uid="{533258F3-EA2C-4CAD-BD74-A5194B5D8935}"/>
+    <hyperlink ref="G51" r:id="rId46" xr:uid="{B5930C01-B6D3-4147-9182-EDAAD2687DE8}"/>
+    <hyperlink ref="G52" r:id="rId47" xr:uid="{B44C98A6-5000-4C5B-B617-FA27A193DBD0}"/>
+    <hyperlink ref="G53" r:id="rId48" xr:uid="{13427CD9-DF27-40D9-A25B-D0B8617B6C76}"/>
+    <hyperlink ref="G54" r:id="rId49" xr:uid="{10A28162-0806-464D-A11E-77CEA45D8B3F}"/>
+    <hyperlink ref="G55" r:id="rId50" xr:uid="{348C2C3C-F347-44FA-AE19-FC3922CE5E15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId29"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM with updated part quantities
</commit_message>
<xml_diff>
--- a/design/electronics/BOM.xlsx
+++ b/design/electronics/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Purdue\ECE47700\DodgeBot\design\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9319E55E-9488-485A-A77D-3691F8F34B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D106F4ED-09F8-4A8D-92CC-413AC2BF2D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Buck Con. Diode</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/VS-6TQ045S-M3/5426222</t>
-  </si>
-  <si>
     <t>GRM2195C1H103JA01D</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
   </si>
   <si>
     <t>What we have to pay:</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kyocera-avx/TPSC107K010R0200/946529</t>
   </si>
   <si>
     <t>3.3V LDO</t>
@@ -535,6 +529,12 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A106KAYNNNE/3888549</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/10SVPC330M/5719731?s=N4IgTCBcDaIIwAYDKA1ACgYQMxYQWQB0AXYkAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/comchip-technology/CDBC520-HF/5226193?s=N4IgTCBcDaIGwBYCMBaJB2AzGNKByAIgDoAupIAugL5A</t>
   </si>
 </sst>
 </file>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,15 +952,15 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -976,7 +976,7 @@
         <v>14.84</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1018,15 +1018,15 @@
         <v>0.35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1039,12 +1039,12 @@
         <v>1.39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1056,19 +1056,19 @@
         <v>0.61</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:E34" si="1">$C6*$D6</f>
+        <f t="shared" ref="E6:E33" si="1">$C6*$D6</f>
         <v>0.61</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1081,15 +1081,15 @@
         <v>1.55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1102,15 +1102,15 @@
         <v>1.86</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1123,15 +1123,15 @@
         <v>0.25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1144,15 +1144,15 @@
         <v>6.7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1165,15 +1165,15 @@
         <v>25.04</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1186,15 +1186,15 @@
         <v>0.69</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1207,15 +1207,15 @@
         <v>0.74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1228,15 +1228,15 @@
         <v>6.42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1249,15 +1249,15 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1270,15 +1270,15 @@
         <v>0.35</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1291,15 +1291,15 @@
         <v>0.53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1312,15 +1312,15 @@
         <v>3.39</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1333,15 +1333,15 @@
         <v>1.72</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1354,15 +1354,15 @@
         <v>17.34</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1375,15 +1375,15 @@
         <v>1.26</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1396,15 +1396,15 @@
         <v>2.68</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1417,15 +1417,15 @@
         <v>1.2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1438,36 +1438,36 @@
         <v>0.88</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
       <c r="C25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" s="3">
         <v>0.12</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1480,15 +1480,15 @@
         <v>0.59</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
         <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1501,15 +1501,15 @@
         <v>0.61</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1522,15 +1522,15 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1543,15 +1543,15 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1564,15 +1564,15 @@
         <v>2.68</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1585,15 +1585,15 @@
         <v>0.13</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1606,15 +1606,15 @@
         <v>0.13</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1627,15 +1627,15 @@
         <v>11.64</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -1644,19 +1644,19 @@
         <v>0.1</v>
       </c>
       <c r="E35" s="3">
-        <f>$C35*$D35</f>
+        <f t="shared" ref="E35:E55" si="2">$C35*$D35</f>
         <v>0.8</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -1665,19 +1665,19 @@
         <v>0.1</v>
       </c>
       <c r="E36" s="3">
-        <f>$C36*$D36</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1686,19 +1686,19 @@
         <v>0.1</v>
       </c>
       <c r="E37" s="3">
-        <f>$C37*$D37</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -1707,19 +1707,19 @@
         <v>0.1</v>
       </c>
       <c r="E38" s="3">
-        <f>$C38*$D38</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1728,40 +1728,40 @@
         <v>0.1</v>
       </c>
       <c r="E39" s="3">
-        <f>$C39*$D39</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E40" s="3">
-        <f>$C40*$D40</f>
-        <v>0.1</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -1770,19 +1770,19 @@
         <v>0.1</v>
       </c>
       <c r="E41" s="3">
-        <f>$C41*$D41</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s">
         <v>136</v>
-      </c>
-      <c r="B42" t="s">
-        <v>138</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -1791,19 +1791,19 @@
         <v>1.33</v>
       </c>
       <c r="E42" s="3">
-        <f>$C42*$D42</f>
+        <f t="shared" si="2"/>
         <v>7.98</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1812,19 +1812,19 @@
         <v>0.1</v>
       </c>
       <c r="E43" s="3">
-        <f>$C43*$D43</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1833,19 +1833,19 @@
         <v>0.1</v>
       </c>
       <c r="E44" s="3">
-        <f>$C44*$D44</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45">
         <v>8</v>
@@ -1854,19 +1854,19 @@
         <v>0.1</v>
       </c>
       <c r="E45" s="3">
-        <f>$C45*$D45</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C46">
         <v>8</v>
@@ -1875,19 +1875,19 @@
         <v>0.1</v>
       </c>
       <c r="E46" s="3">
-        <f>$C46*$D46</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -1896,19 +1896,19 @@
         <v>0.1</v>
       </c>
       <c r="E47" s="3">
-        <f>$C47*$D47</f>
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48">
         <v>29</v>
@@ -1917,19 +1917,19 @@
         <v>2.7E-2</v>
       </c>
       <c r="E48" s="3">
-        <f>$C48*$D48</f>
+        <f t="shared" si="2"/>
         <v>0.78300000000000003</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1938,19 +1938,19 @@
         <v>0.1</v>
       </c>
       <c r="E49" s="3">
-        <f>$C49*$D49</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C50">
         <v>10</v>
@@ -1959,19 +1959,19 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E50" s="3">
-        <f>$C50*$D50</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1980,19 +1980,19 @@
         <v>0.23</v>
       </c>
       <c r="E51" s="3">
-        <f>$C51*$D51</f>
+        <f t="shared" si="2"/>
         <v>0.69000000000000006</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -2001,19 +2001,19 @@
         <v>0.27</v>
       </c>
       <c r="E52" s="3">
-        <f>$C52*$D52</f>
+        <f t="shared" si="2"/>
         <v>0.81</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2022,19 +2022,19 @@
         <v>0.1</v>
       </c>
       <c r="E53" s="3">
-        <f>$C53*$D53</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2043,19 +2043,19 @@
         <v>0.1</v>
       </c>
       <c r="E54" s="3">
-        <f>$C54*$D54</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2064,29 +2064,29 @@
         <v>0.18</v>
       </c>
       <c r="E55" s="3">
-        <f>$C55*$D55</f>
+        <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F59" s="3">
         <f>SUM($E2:$E55)</f>
-        <v>134.113</v>
+        <v>134.35299999999998</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F60" s="3">
         <f>$F$59-$E$10-$E$11-$E$22-$E$23</f>
-        <v>98.492999999999981</v>
+        <v>98.732999999999961</v>
       </c>
     </row>
   </sheetData>
@@ -2141,8 +2141,11 @@
     <hyperlink ref="G53" r:id="rId48" xr:uid="{13427CD9-DF27-40D9-A25B-D0B8617B6C76}"/>
     <hyperlink ref="G54" r:id="rId49" xr:uid="{10A28162-0806-464D-A11E-77CEA45D8B3F}"/>
     <hyperlink ref="G55" r:id="rId50" xr:uid="{348C2C3C-F347-44FA-AE19-FC3922CE5E15}"/>
+    <hyperlink ref="G15" r:id="rId51" xr:uid="{46950DA7-84BE-471C-A4CF-C3A27ED94D5A}"/>
+    <hyperlink ref="G16" r:id="rId52" xr:uid="{D6D82FBD-4014-4298-997B-4B560C46B68B}"/>
+    <hyperlink ref="G17" r:id="rId53" xr:uid="{F83DAAB3-2185-4223-85A1-6330871B7D5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId51"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>